<commit_message>
Added date/datetime support to excel parser
</commit_message>
<xml_diff>
--- a/src/test/resources/test_data/with_types.xlsx
+++ b/src/test/resources/test_data/with_types.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">some_double</t>
   </si>
@@ -29,6 +29,12 @@
   </si>
   <si>
     <t xml:space="preserve">some_time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some_date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some_datetime</t>
   </si>
   <si>
     <t xml:space="preserve">hello</t>
@@ -41,9 +47,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="HH:MM:SS\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="HH:MM"/>
+    <numFmt numFmtId="166" formatCode="D/M/YY"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YYYY\ HH:MM:SS"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -110,7 +118,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -119,7 +127,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -140,50 +156,71 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.9081632653061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="22.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="s">
-        <v>3</v>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="n">
         <v>0.437615740740741</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="3" t="n">
+        <v>40461</v>
+      </c>
+      <c r="E2" s="4" t="n">
+        <v>40461.4376157407</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>4</v>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
       </c>
       <c r="C3" s="2" t="n">
         <v>0.319444444444444</v>
+      </c>
+      <c r="D3" s="3" t="n">
+        <v>40483</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>40483.3194444444</v>
       </c>
     </row>
   </sheetData>

</xml_diff>